<commit_message>
Add area and efficiency
</commit_message>
<xml_diff>
--- a/dataset_temporary version_0227/PV generation dataset/Area for with optimizer.xlsx
+++ b/dataset_temporary version_0227/PV generation dataset/Area for with optimizer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hkustconnect-my.sharepoint.com/personal/lcchanaj_connect_ust_hk/Documents/桌面/FYP Code/dataset_temporary version_0227/PV generation dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="11_AD4DBB64A54DDB1B405E381765D817954F90DF24" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04AB03EC-672C-49DF-A85A-E8D3609CD4FD}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="11_AD4DBB64A54DDB1B405E381765D817954F90DF24" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FAC94AF-F3A7-4DC5-9F20-3547FE2042F8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -511,14 +511,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.625" customWidth="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="2" max="2" width="30.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.35">
@@ -810,5 +810,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>